<commit_message>
create items.cs and attributes.cs
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items.xlsx
+++ b/Assets/Resources/Items.xlsx
@@ -48,22 +48,22 @@
     <t>BulletNumber++</t>
   </si>
   <si>
-    <t>BulletAdvance++</t>
-  </si>
-  <si>
-    <t>Energy++</t>
-  </si>
-  <si>
-    <t>EnergyMax++</t>
-  </si>
-  <si>
-    <t>AutoEnergy++</t>
+    <t>BulletLevel++</t>
   </si>
   <si>
     <t>MoveSpeed++</t>
   </si>
   <si>
     <t>BulletSpeed</t>
+  </si>
+  <si>
+    <t>Deffend</t>
+  </si>
+  <si>
+    <t>Lazer Gun</t>
+  </si>
+  <si>
+    <t>Solar Panel</t>
   </si>
 </sst>
 </file>
@@ -994,32 +994,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="11.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="38.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="23.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="13.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="23.5555555555556" customWidth="1"/>
     <col min="5" max="5" width="13.2222222222222" customWidth="1"/>
-    <col min="6" max="6" width="15.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="9.88888888888889" customWidth="1"/>
     <col min="7" max="7" width="20.8888888888889" customWidth="1"/>
     <col min="8" max="8" width="12.4444444444444" customWidth="1"/>
     <col min="9" max="9" width="14.7777777777778" customWidth="1"/>
     <col min="10" max="10" width="19.2222222222222" customWidth="1"/>
-    <col min="11" max="11" width="14.1111111111111" customWidth="1"/>
-    <col min="12" max="12" width="18.5555555555556" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="13.8888888888889" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13.8888888888889" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1059,16 +1056,87 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>